<commit_message>
v2.0.05061200 long press send pulse
</commit_message>
<xml_diff>
--- a/arduino/工作簿1.xlsx
+++ b/arduino/工作簿1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tongjieducn-my.sharepoint.com/personal/dragonroll_tongji_edu_cn/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tongjieducn-my.sharepoint.com/personal/dragonroll_tongji_edu_cn/Documents/Projects/210228PulseBeeper/arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B88A6A6A-FE5D-4F7F-8EB9-903C7C3BC07A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{B88A6A6A-FE5D-4F7F-8EB9-903C7C3BC07A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BEEBCA67-8A88-45E7-BC99-C98FE2A79FBC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{91CEC2E2-ACD5-40E4-A827-6F828CC113C0}"/>
+    <workbookView xWindow="-10725" yWindow="2760" windowWidth="21600" windowHeight="11835" xr2:uid="{91CEC2E2-ACD5-40E4-A827-6F828CC113C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA6FE50-8245-4FA0-8D17-AD2273AA0A7C}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -411,23 +407,32 @@
       <c r="E1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>26</v>
       </c>
@@ -435,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -443,7 +448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>28</v>
       </c>
@@ -451,7 +456,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>25</v>
       </c>
@@ -459,27 +464,32 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>25</v>
       </c>
@@ -495,8 +505,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0</v>
       </c>

</xml_diff>